<commit_message>
switch to updated QUEST categorisations
</commit_message>
<xml_diff>
--- a/data-export/export_202108/macro-sum_quarterly.xlsx
+++ b/data-export/export_202108/macro-sum_quarterly.xlsx
@@ -849,13 +849,13 @@
         </is>
       </c>
       <c r="E10">
-        <v>6890632771.922575</v>
+        <v>6838101438.21</v>
       </c>
       <c r="F10">
-        <v>5916517298.793182</v>
+        <v>5881087738.91</v>
       </c>
       <c r="G10">
-        <v>7260548.954392636</v>
+        <v>1993918.92</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -870,13 +870,13 @@
         <v>4</v>
       </c>
       <c r="L10">
-        <v>32703857.885</v>
+        <v>20868714.09</v>
       </c>
       <c r="M10">
-        <v>2.328306436538696e-10</v>
+        <v>-6.984919309616089e-10</v>
       </c>
       <c r="N10">
-        <v>974115473.1293925</v>
+        <v>957013699.3</v>
       </c>
     </row>
     <row r="11">
@@ -999,13 +999,13 @@
         </is>
       </c>
       <c r="E13">
-        <v>1431544126.304155</v>
+        <v>1465588315.71673</v>
       </c>
       <c r="F13">
-        <v>1208320460.852372</v>
+        <v>1237098020.230555</v>
       </c>
       <c r="G13">
-        <v>197681733.996095</v>
+        <v>202948364.0304877</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1026,7 +1026,7 @@
         <v>284418.1699999999</v>
       </c>
       <c r="N13">
-        <v>223223665.4517827</v>
+        <v>228490295.4861753</v>
       </c>
     </row>
     <row r="14">
@@ -1089,10 +1089,10 @@
         </is>
       </c>
       <c r="E15">
-        <v>26644982.75</v>
+        <v>26247019.75</v>
       </c>
       <c r="F15">
-        <v>11381038.68</v>
+        <v>11102464.58</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1110,13 +1110,13 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <v>15263944.07</v>
+        <v>15144555.17</v>
       </c>
       <c r="M15">
         <v>4.656612873077393e-10</v>
       </c>
       <c r="N15">
-        <v>15263944.07</v>
+        <v>15144555.17</v>
       </c>
     </row>
     <row r="16">
@@ -1189,10 +1189,10 @@
         </is>
       </c>
       <c r="E17">
-        <v>4033513868.82</v>
+        <v>4023993108.01</v>
       </c>
       <c r="F17">
-        <v>1648706245.24</v>
+        <v>1642041712.72</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1210,13 +1210,13 @@
         <v>0</v>
       </c>
       <c r="L17">
-        <v>2384807623.58</v>
+        <v>2381951395.29</v>
       </c>
       <c r="M17">
-        <v>-7.275957614183426e-11</v>
+        <v>1.309672370553017e-10</v>
       </c>
       <c r="N17">
-        <v>2384807623.58</v>
+        <v>2381951395.29</v>
       </c>
     </row>
     <row r="18">
@@ -1239,13 +1239,13 @@
         </is>
       </c>
       <c r="E18">
-        <v>546640379.64</v>
+        <v>502727459.03</v>
       </c>
       <c r="F18">
-        <v>251637594.47</v>
+        <v>214548988.59</v>
       </c>
       <c r="G18">
-        <v>4003249.32</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1254,19 +1254,19 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>290706716.95</v>
+        <v>288178470.44</v>
       </c>
       <c r="M18">
-        <v>2621804.900000005</v>
+        <v>3.899913281202316e-09</v>
       </c>
       <c r="N18">
-        <v>295002785.17</v>
+        <v>288178470.44</v>
       </c>
     </row>
     <row r="19">
@@ -1289,10 +1289,10 @@
         </is>
       </c>
       <c r="E19">
-        <v>2157845706.08</v>
+        <v>2154211756.32</v>
       </c>
       <c r="F19">
-        <v>856998799.74</v>
+        <v>854455034.9400001</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1310,13 +1310,13 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>1300846906.34</v>
+        <v>1299756721.38</v>
       </c>
       <c r="M19">
-        <v>-5.835318006575108e-09</v>
+        <v>-5.951733328402042e-09</v>
       </c>
       <c r="N19">
-        <v>1299280963.11</v>
+        <v>1298190778.15</v>
       </c>
     </row>
     <row r="20">
@@ -1389,34 +1389,34 @@
         </is>
       </c>
       <c r="E21">
-        <v>410190192.75</v>
+        <v>366058141.99</v>
       </c>
       <c r="F21">
-        <v>200624187.12</v>
+        <v>169428784.83</v>
       </c>
       <c r="G21">
-        <v>3531838.11</v>
+        <v>969325.1</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>196848239.88</v>
+        <v>194388815.27</v>
       </c>
       <c r="M21">
-        <v>7465030.8</v>
+        <v>2.473825588822365e-10</v>
       </c>
       <c r="N21">
-        <v>209566005.63</v>
+        <v>196629357.16</v>
       </c>
     </row>
     <row r="22">
@@ -1439,34 +1439,34 @@
         </is>
       </c>
       <c r="E22">
-        <v>8351245901.727885</v>
+        <v>8703630252.397884</v>
       </c>
       <c r="F22">
-        <v>6916630336.032767</v>
+        <v>7171417010.572767</v>
       </c>
       <c r="G22">
-        <v>1199624599.480042</v>
+        <v>1209989577.310042</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="J22">
-        <v>179.6600000009747</v>
+        <v>218.6600000009747</v>
       </c>
       <c r="K22">
         <v>4</v>
       </c>
       <c r="L22">
-        <v>114548326.7864868</v>
+        <v>163734851.3064868</v>
       </c>
       <c r="M22">
-        <v>78471965.18000001</v>
+        <v>103679600.79</v>
       </c>
       <c r="N22">
-        <v>1434615565.695117</v>
+        <v>1532213241.825117</v>
       </c>
     </row>
     <row r="23">
@@ -1539,34 +1539,34 @@
         </is>
       </c>
       <c r="E24">
-        <v>32449042612.08852</v>
+        <v>29719112845.94</v>
       </c>
       <c r="F24">
-        <v>26077744446.3335</v>
+        <v>24714452706.34</v>
       </c>
       <c r="G24">
-        <v>137929141.1892286</v>
+        <v>106250046.96</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="J24">
-        <v>1147</v>
+        <v>1094</v>
       </c>
       <c r="K24">
         <v>35</v>
       </c>
       <c r="L24">
-        <v>2006288620.225</v>
+        <v>720551948.01</v>
       </c>
       <c r="M24">
-        <v>30365769.71999999</v>
+        <v>5158134.110000004</v>
       </c>
       <c r="N24">
-        <v>6371298165.755019</v>
+        <v>5004660139.6</v>
       </c>
     </row>
     <row r="25">
@@ -1639,10 +1639,10 @@
         </is>
       </c>
       <c r="E26">
-        <v>3559172097.215</v>
+        <v>4386665103.635</v>
       </c>
       <c r="F26">
-        <v>2198889699.96</v>
+        <v>2615831783.2</v>
       </c>
       <c r="G26">
         <v>193996454.505</v>
@@ -1651,7 +1651,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -1660,13 +1660,13 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <v>1166285942.75</v>
+        <v>1569762085.17</v>
       </c>
       <c r="M26">
-        <v>192470711.335</v>
+        <v>199545492.095</v>
       </c>
       <c r="N26">
-        <v>1360282397.255</v>
+        <v>1770833320.435</v>
       </c>
     </row>
     <row r="27">
@@ -1739,34 +1739,34 @@
         </is>
       </c>
       <c r="E28">
-        <v>3310490864.323594</v>
+        <v>3914040508.977115</v>
       </c>
       <c r="F28">
-        <v>2771055565.818731</v>
+        <v>3193541743.922233</v>
       </c>
       <c r="G28">
-        <v>453283520.8607293</v>
+        <v>481163399.5899578</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J28">
-        <v>112.3399999990253</v>
+        <v>129.3399999990253</v>
       </c>
       <c r="K28">
         <v>12</v>
       </c>
       <c r="L28">
-        <v>11670210.15351325</v>
+        <v>152544963.0535133</v>
       </c>
       <c r="M28">
-        <v>11418840.16999999</v>
+        <v>14430895.10999999</v>
       </c>
       <c r="N28">
-        <v>539435298.504863</v>
+        <v>720498765.0548826</v>
       </c>
     </row>
     <row r="29">
@@ -1879,10 +1879,10 @@
         </is>
       </c>
       <c r="E31">
-        <v>50929303.115</v>
+        <v>45484795.3</v>
       </c>
       <c r="F31">
-        <v>22024952.105</v>
+        <v>18852861.76</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1891,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -1900,13 +1900,13 @@
         <v>0</v>
       </c>
       <c r="L31">
-        <v>27626220.775</v>
+        <v>26631933.54</v>
       </c>
       <c r="M31">
-        <v>1278130.234999999</v>
+        <v>-4.656612873077393e-10</v>
       </c>
       <c r="N31">
-        <v>28904351.01</v>
+        <v>26631933.54</v>
       </c>
     </row>
     <row r="32">
@@ -1979,10 +1979,10 @@
         </is>
       </c>
       <c r="E33">
-        <v>8458067453.06</v>
+        <v>8434293013.08</v>
       </c>
       <c r="F33">
-        <v>3417449336.51</v>
+        <v>3402442913.1</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1991,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J33">
         <v>0</v>
@@ -2000,13 +2000,13 @@
         <v>0</v>
       </c>
       <c r="L33">
-        <v>5035346759.55</v>
+        <v>5029850111.98</v>
       </c>
       <c r="M33">
-        <v>3271368.999999999</v>
+        <v>-8.146798791131005e-10</v>
       </c>
       <c r="N33">
-        <v>5040618116.55</v>
+        <v>5031850099.98</v>
       </c>
     </row>
     <row r="34">
@@ -2029,34 +2029,34 @@
         </is>
       </c>
       <c r="E34">
-        <v>912225590.485</v>
+        <v>643491710.0600001</v>
       </c>
       <c r="F34">
-        <v>501788285.775</v>
+        <v>278814863.9</v>
       </c>
       <c r="G34">
-        <v>22881511.82</v>
+        <v>0</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
       <c r="L34">
-        <v>379163656.045</v>
+        <v>364676846.16</v>
       </c>
       <c r="M34">
-        <v>18769584.485</v>
+        <v>4.365574568510056e-10</v>
       </c>
       <c r="N34">
-        <v>410437304.71</v>
+        <v>364676846.16</v>
       </c>
     </row>
     <row r="35">
@@ -2079,10 +2079,10 @@
         </is>
       </c>
       <c r="E35">
-        <v>2380912963.6</v>
+        <v>2370611729.71</v>
       </c>
       <c r="F35">
-        <v>941981129.84</v>
+        <v>935820840.25</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -2091,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J35">
         <v>0</v>
@@ -2100,13 +2100,13 @@
         <v>0</v>
       </c>
       <c r="L35">
-        <v>1436578889.41</v>
+        <v>1434539093.31</v>
       </c>
       <c r="M35">
-        <v>2101148.199999998</v>
+        <v>-9.313225746154785e-10</v>
       </c>
       <c r="N35">
-        <v>1438931833.76</v>
+        <v>1434790889.46</v>
       </c>
     </row>
     <row r="36">
@@ -2179,34 +2179,34 @@
         </is>
       </c>
       <c r="E37">
-        <v>1471955786.53</v>
+        <v>986985646.04</v>
       </c>
       <c r="F37">
-        <v>867849704.92</v>
+        <v>487856781.73</v>
       </c>
       <c r="G37">
-        <v>30042264.79</v>
+        <v>7063094.88</v>
       </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="I37">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="J37">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K37">
         <v>0</v>
       </c>
       <c r="L37">
-        <v>485777563.8</v>
+        <v>471298980.65</v>
       </c>
       <c r="M37">
-        <v>55400765.90000001</v>
+        <v>16770285.96</v>
       </c>
       <c r="N37">
-        <v>604106081.61</v>
+        <v>499128864.31</v>
       </c>
     </row>
     <row r="38">
@@ -2229,34 +2229,34 @@
         </is>
       </c>
       <c r="E38">
-        <v>14027414495.49244</v>
+        <v>21246222056.13244</v>
       </c>
       <c r="F38">
-        <v>11494276870.32086</v>
+        <v>17361355258.90086</v>
       </c>
       <c r="G38">
-        <v>1995884198.560849</v>
+        <v>2585300491.020849</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38">
-        <v>568</v>
+        <v>745</v>
       </c>
       <c r="J38">
-        <v>366.8800000011905</v>
+        <v>742.8800000011905</v>
       </c>
       <c r="K38">
-        <v>64.66000000034843</v>
+        <v>104.6600000003484</v>
       </c>
       <c r="L38">
-        <v>267618706.0558994</v>
+        <v>513995554.2858995</v>
       </c>
       <c r="M38">
-        <v>250641303.97</v>
+        <v>521272802.51</v>
       </c>
       <c r="N38">
-        <v>2533137625.171581</v>
+        <v>3884866797.231581</v>
       </c>
     </row>
     <row r="39">
@@ -2329,34 +2329,34 @@
         </is>
       </c>
       <c r="E40">
-        <v>60803938165.68874</v>
+        <v>45394414047.615</v>
       </c>
       <c r="F40">
-        <v>45393696883.21193</v>
+        <v>34969990234.875</v>
       </c>
       <c r="G40">
-        <v>1422974771.492563</v>
+        <v>671651355.11</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40">
-        <v>542</v>
+        <v>340</v>
       </c>
       <c r="J40">
-        <v>3423</v>
+        <v>3007</v>
       </c>
       <c r="K40">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="L40">
-        <v>7373851155.955</v>
+        <v>3751439763.78</v>
       </c>
       <c r="M40">
-        <v>492285757.89</v>
+        <v>221654259.35</v>
       </c>
       <c r="N40">
-        <v>15410241282.47682</v>
+        <v>10424423812.74</v>
       </c>
     </row>
     <row r="41">
@@ -2429,10 +2429,10 @@
         </is>
       </c>
       <c r="E42">
-        <v>9693659441.355</v>
+        <v>12031468561.875</v>
       </c>
       <c r="F42">
-        <v>5872374225.805</v>
+        <v>7047506732.455</v>
       </c>
       <c r="G42">
         <v>746988725.225</v>
@@ -2441,7 +2441,7 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -2450,13 +2450,13 @@
         <v>17</v>
       </c>
       <c r="L42">
-        <v>3068197064.245</v>
+        <v>4182571434.815</v>
       </c>
       <c r="M42">
-        <v>662736334.885</v>
+        <v>711038578.1850001</v>
       </c>
       <c r="N42">
-        <v>3821285215.55</v>
+        <v>4983961829.42</v>
       </c>
     </row>
     <row r="43">
@@ -2529,34 +2529,34 @@
         </is>
       </c>
       <c r="E44">
-        <v>4093942249.208814</v>
+        <v>8188630293.72756</v>
       </c>
       <c r="F44">
-        <v>3465890745.852211</v>
+        <v>6671047664.239141</v>
       </c>
       <c r="G44">
-        <v>501469839.0965887</v>
+        <v>709237644.7491511</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="J44">
-        <v>419.1199999988095</v>
+        <v>479.1199999988095</v>
       </c>
       <c r="K44">
-        <v>39.33999999965157</v>
+        <v>45.33999999965157</v>
       </c>
       <c r="L44">
-        <v>19446195.99410056</v>
+        <v>570802881.4441005</v>
       </c>
       <c r="M44">
-        <v>16757715.18</v>
+        <v>32506183.73999997</v>
       </c>
       <c r="N44">
-        <v>628051503.3566027</v>
+        <v>1517582629.488419</v>
       </c>
     </row>
     <row r="45">
@@ -2629,10 +2629,10 @@
         </is>
       </c>
       <c r="E46">
-        <v>98681279.69</v>
+        <v>89906937.81</v>
       </c>
       <c r="F46">
-        <v>41549238.16</v>
+        <v>37162067.23</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -2641,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -2650,13 +2650,13 @@
         <v>0</v>
       </c>
       <c r="L46">
-        <v>53622304.78</v>
+        <v>52744870.58</v>
       </c>
       <c r="M46">
-        <v>3509736.75</v>
+        <v>1.164153218269348e-10</v>
       </c>
       <c r="N46">
-        <v>57132041.53</v>
+        <v>52744870.58</v>
       </c>
     </row>
     <row r="47">
@@ -2729,10 +2729,10 @@
         </is>
       </c>
       <c r="E48">
-        <v>5237865356.15</v>
+        <v>5200583894.62</v>
       </c>
       <c r="F48">
-        <v>2164839641.84</v>
+        <v>2143892983</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2741,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J48">
         <v>0</v>
@@ -2750,13 +2750,13 @@
         <v>0</v>
       </c>
       <c r="L48">
-        <v>3062724985.97</v>
+        <v>3056690911.62</v>
       </c>
       <c r="M48">
-        <v>10300728.34000003</v>
+        <v>2.731394488364458e-08</v>
       </c>
       <c r="N48">
-        <v>3073025714.31</v>
+        <v>3056690911.62</v>
       </c>
     </row>
     <row r="49">
@@ -2779,34 +2779,34 @@
         </is>
       </c>
       <c r="E49">
-        <v>991759642.29</v>
+        <v>296335400.8</v>
       </c>
       <c r="F49">
-        <v>715665502.01</v>
+        <v>136133465.47</v>
       </c>
       <c r="G49">
-        <v>55853362.37</v>
+        <v>0</v>
       </c>
       <c r="H49">
         <v>0</v>
       </c>
       <c r="I49">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="J49">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="K49">
         <v>0</v>
       </c>
       <c r="L49">
-        <v>186224774.64</v>
+        <v>160201935.33</v>
       </c>
       <c r="M49">
-        <v>43676742.03</v>
+        <v>-1.527951098978519e-09</v>
       </c>
       <c r="N49">
-        <v>276094140.28</v>
+        <v>160201935.33</v>
       </c>
     </row>
     <row r="50">
@@ -2829,10 +2829,10 @@
         </is>
       </c>
       <c r="E50">
-        <v>1978040354.44</v>
+        <v>1955335496.62</v>
       </c>
       <c r="F50">
-        <v>769755923.83</v>
+        <v>756682028.89</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2841,7 +2841,7 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -2850,13 +2850,13 @@
         <v>0</v>
       </c>
       <c r="L50">
-        <v>1202645419.65</v>
+        <v>1198653467.73</v>
       </c>
       <c r="M50">
-        <v>5639010.959999997</v>
+        <v>-3.12138581648469e-09</v>
       </c>
       <c r="N50">
-        <v>1208284430.61</v>
+        <v>1198653467.73</v>
       </c>
     </row>
     <row r="51">
@@ -2929,34 +2929,34 @@
         </is>
       </c>
       <c r="E52">
-        <v>2066649806.62</v>
+        <v>1093543617.23</v>
       </c>
       <c r="F52">
-        <v>1348212616.18</v>
+        <v>580846866.17</v>
       </c>
       <c r="G52">
-        <v>67289867.81</v>
+        <v>7805171.57</v>
       </c>
       <c r="H52">
         <v>0</v>
       </c>
       <c r="I52">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="J52">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K52">
         <v>0</v>
       </c>
       <c r="L52">
-        <v>483076150.61</v>
+        <v>451516261.17</v>
       </c>
       <c r="M52">
-        <v>133276749.67</v>
+        <v>51026817.37</v>
       </c>
       <c r="N52">
-        <v>718437190.4399999</v>
+        <v>512696751.06</v>
       </c>
     </row>
     <row r="53">
@@ -2979,34 +2979,34 @@
         </is>
       </c>
       <c r="E53">
-        <v>13524854514.86944</v>
+        <v>24959599412.83944</v>
       </c>
       <c r="F53">
-        <v>11122801559.21566</v>
+        <v>20672173988.49566</v>
       </c>
       <c r="G53">
-        <v>1915921767.85803</v>
+        <v>2697813925.56803</v>
       </c>
       <c r="H53">
         <v>0</v>
       </c>
       <c r="I53">
-        <v>604</v>
+        <v>920</v>
       </c>
       <c r="J53">
-        <v>552.0500000007031</v>
+        <v>1285.050000000703</v>
       </c>
       <c r="K53">
-        <v>172.6600000003484</v>
+        <v>215.6600000003484</v>
       </c>
       <c r="L53">
-        <v>225145747.8741641</v>
+        <v>463809157.4341642</v>
       </c>
       <c r="M53">
-        <v>251269728.33</v>
+        <v>662590794.4499999</v>
       </c>
       <c r="N53">
-        <v>2402052955.65378</v>
+        <v>4287425424.34378</v>
       </c>
     </row>
     <row r="54">
@@ -3079,34 +3079,34 @@
         </is>
       </c>
       <c r="E55">
-        <v>65978114513.09763</v>
+        <v>46284485577.76</v>
       </c>
       <c r="F55">
-        <v>49777781539.9868</v>
+        <v>34997534129.235</v>
       </c>
       <c r="G55">
-        <v>1779848053.210778</v>
+        <v>751082175.8099999</v>
       </c>
       <c r="H55">
         <v>0</v>
       </c>
       <c r="I55">
-        <v>779.5</v>
+        <v>426.5</v>
       </c>
       <c r="J55">
-        <v>3633</v>
+        <v>2775</v>
       </c>
       <c r="K55">
-        <v>141</v>
+        <v>94</v>
       </c>
       <c r="L55">
-        <v>6980126032.41</v>
+        <v>4099820936.12</v>
       </c>
       <c r="M55">
-        <v>563315496.88</v>
+        <v>151994430.76</v>
       </c>
       <c r="N55">
-        <v>16200332973.11083</v>
+        <v>11286951448.525</v>
       </c>
     </row>
     <row r="56">
@@ -3179,10 +3179,10 @@
         </is>
       </c>
       <c r="E57">
-        <v>10394314143.835</v>
+        <v>12148765119.545</v>
       </c>
       <c r="F57">
-        <v>6422000375.29</v>
+        <v>7306501070.29</v>
       </c>
       <c r="G57">
         <v>828169675.3049999</v>
@@ -3191,7 +3191,7 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="J57">
         <v>0</v>
@@ -3200,13 +3200,13 @@
         <v>116.5</v>
       </c>
       <c r="L57">
-        <v>3054101201.05</v>
+        <v>3825839470.39</v>
       </c>
       <c r="M57">
-        <v>460622854.605</v>
+        <v>558834865.975</v>
       </c>
       <c r="N57">
-        <v>3972313768.545</v>
+        <v>4842264049.255</v>
       </c>
     </row>
     <row r="58">
@@ -3279,34 +3279,34 @@
         </is>
       </c>
       <c r="E59">
-        <v>5105633280.962932</v>
+        <v>11311749548.75556</v>
       </c>
       <c r="F59">
-        <v>4384426411.332542</v>
+        <v>9436165151.159342</v>
       </c>
       <c r="G59">
-        <v>558599342.2311925</v>
+        <v>920811120.5319703</v>
       </c>
       <c r="H59">
         <v>0</v>
       </c>
       <c r="I59">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="J59">
-        <v>728.9499999992969</v>
+        <v>882.9499999992969</v>
       </c>
       <c r="K59">
-        <v>72.33999999965157</v>
+        <v>76.33999999965157</v>
       </c>
       <c r="L59">
-        <v>32898444.49583585</v>
+        <v>615621223.0358359</v>
       </c>
       <c r="M59">
-        <v>20178475.72</v>
+        <v>67342614.72999996</v>
       </c>
       <c r="N59">
-        <v>721206869.6303892</v>
+        <v>1875584397.59622</v>
       </c>
     </row>
     <row r="60">
@@ -3419,10 +3419,10 @@
         </is>
       </c>
       <c r="E62">
-        <v>648080533.225</v>
+        <v>641008694.84</v>
       </c>
       <c r="F62">
-        <v>290714936.585</v>
+        <v>287179017.4</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -3431,7 +3431,7 @@
         <v>0</v>
       </c>
       <c r="I62">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="J62">
         <v>0</v>
@@ -3440,13 +3440,13 @@
         <v>0</v>
       </c>
       <c r="L62">
-        <v>354536861.29</v>
+        <v>353829677.44</v>
       </c>
       <c r="M62">
-        <v>2828735.349999997</v>
+        <v>-2.211891114711761e-09</v>
       </c>
       <c r="N62">
-        <v>357365596.64</v>
+        <v>353829677.44</v>
       </c>
     </row>
     <row r="63">
@@ -3519,10 +3519,10 @@
         </is>
       </c>
       <c r="E64">
-        <v>6695253973.308</v>
+        <v>6663019289.258</v>
       </c>
       <c r="F64">
-        <v>2904512407.064</v>
+        <v>2886492346.554</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -3531,7 +3531,7 @@
         <v>0</v>
       </c>
       <c r="I64">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J64">
         <v>0</v>
@@ -3540,13 +3540,13 @@
         <v>0</v>
       </c>
       <c r="L64">
-        <v>3781653129.684</v>
+        <v>3776526942.704</v>
       </c>
       <c r="M64">
-        <v>9088436.560000004</v>
+        <v>3.059540176764131e-09</v>
       </c>
       <c r="N64">
-        <v>3790741566.244</v>
+        <v>3776526942.704</v>
       </c>
     </row>
     <row r="65">
@@ -3569,34 +3569,34 @@
         </is>
       </c>
       <c r="E65">
-        <v>1968296522.725</v>
+        <v>718779112.2</v>
       </c>
       <c r="F65">
-        <v>1390859130.105</v>
+        <v>336655485.13</v>
       </c>
       <c r="G65">
-        <v>101033883.83</v>
+        <v>0</v>
       </c>
       <c r="H65">
         <v>0</v>
       </c>
       <c r="I65">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="J65">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K65">
         <v>0</v>
       </c>
       <c r="L65">
-        <v>435492972.99</v>
+        <v>382123627.07</v>
       </c>
       <c r="M65">
-        <v>71383604.03000002</v>
+        <v>-1.920852810144424e-09</v>
       </c>
       <c r="N65">
-        <v>577437392.62</v>
+        <v>382123627.07</v>
       </c>
     </row>
     <row r="66">
@@ -3619,10 +3619,10 @@
         </is>
       </c>
       <c r="E66">
-        <v>1330272285.02</v>
+        <v>1315017975.98</v>
       </c>
       <c r="F66">
-        <v>559115313.59</v>
+        <v>550132954.67</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -3631,7 +3631,7 @@
         <v>0</v>
       </c>
       <c r="I66">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J66">
         <v>0</v>
@@ -3640,13 +3640,13 @@
         <v>0</v>
       </c>
       <c r="L66">
-        <v>767765656.7</v>
+        <v>764885021.3099999</v>
       </c>
       <c r="M66">
-        <v>3391314.730000006</v>
+        <v>6.035406840965152e-09</v>
       </c>
       <c r="N66">
-        <v>771156971.4299999</v>
+        <v>764885021.3099999</v>
       </c>
     </row>
     <row r="67">
@@ -3719,34 +3719,34 @@
         </is>
       </c>
       <c r="E68">
-        <v>3457998043.07</v>
+        <v>1288237783.89</v>
       </c>
       <c r="F68">
-        <v>2460348447.34</v>
+        <v>675965552.2</v>
       </c>
       <c r="G68">
-        <v>154546586.08</v>
+        <v>8973517.83</v>
       </c>
       <c r="H68">
         <v>0</v>
       </c>
       <c r="I68">
-        <v>114</v>
+        <v>23</v>
       </c>
       <c r="J68">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="K68">
         <v>0</v>
       </c>
       <c r="L68">
-        <v>605234388.34</v>
+        <v>556349286.47</v>
       </c>
       <c r="M68">
-        <v>135147375.75</v>
+        <v>38012310.4</v>
       </c>
       <c r="N68">
-        <v>997649595.73</v>
+        <v>612272231.6899999</v>
       </c>
     </row>
     <row r="69">
@@ -3769,34 +3769,34 @@
         </is>
       </c>
       <c r="E69">
-        <v>15460632616.86815</v>
+        <v>23942068816.26815</v>
       </c>
       <c r="F69">
-        <v>12605574149.45547</v>
+        <v>19676491074.95547</v>
       </c>
       <c r="G69">
-        <v>2293730921.636453</v>
+        <v>2880612805.556452</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
       <c r="I69">
-        <v>795.7599999996229</v>
+        <v>965.7599999996229</v>
       </c>
       <c r="J69">
-        <v>593.6100000001079</v>
+        <v>1326.610000000108</v>
       </c>
       <c r="K69">
-        <v>364.6600000003484</v>
+        <v>426.6600000003484</v>
       </c>
       <c r="L69">
-        <v>215706983.5576848</v>
+        <v>421452912.1776848</v>
       </c>
       <c r="M69">
-        <v>218560398.17</v>
+        <v>613164632.1999999</v>
       </c>
       <c r="N69">
-        <v>2855058467.41268</v>
+        <v>4265577741.31268</v>
       </c>
     </row>
     <row r="70">
@@ -3869,34 +3869,34 @@
         </is>
       </c>
       <c r="E71">
-        <v>74676294509.79555</v>
+        <v>58535884803.495</v>
       </c>
       <c r="F71">
-        <v>56134353331.77065</v>
+        <v>44555437338.085</v>
       </c>
       <c r="G71">
-        <v>1759727460.964494</v>
+        <v>909006132.125</v>
       </c>
       <c r="H71">
         <v>0</v>
       </c>
       <c r="I71">
-        <v>619.5</v>
+        <v>418.5</v>
       </c>
       <c r="J71">
-        <v>3115</v>
+        <v>2347</v>
       </c>
       <c r="K71">
-        <v>205</v>
+        <v>127</v>
       </c>
       <c r="L71">
-        <v>8605662367.77</v>
+        <v>5682492217.19</v>
       </c>
       <c r="M71">
-        <v>556627942.63</v>
+        <v>162023708.6000001</v>
       </c>
       <c r="N71">
-        <v>18541941178.02489</v>
+        <v>13980447465.41</v>
       </c>
     </row>
     <row r="72">
@@ -3969,10 +3969,10 @@
         </is>
       </c>
       <c r="E73">
-        <v>13328918087.091</v>
+        <v>15313815879.311</v>
       </c>
       <c r="F73">
-        <v>8368570732.148</v>
+        <v>9366832221.988001</v>
       </c>
       <c r="G73">
         <v>1091896671.76</v>
@@ -3981,7 +3981,7 @@
         <v>0</v>
       </c>
       <c r="I73">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -3990,13 +3990,13 @@
         <v>174</v>
       </c>
       <c r="L73">
-        <v>3690228044.288</v>
+        <v>4586260460.958</v>
       </c>
       <c r="M73">
-        <v>485878823.6999999</v>
+        <v>576482709.41</v>
       </c>
       <c r="N73">
-        <v>4960347354.943</v>
+        <v>5946983657.323</v>
       </c>
     </row>
     <row r="74">
@@ -4069,34 +4069,34 @@
         </is>
       </c>
       <c r="E75">
-        <v>5473988105.926305</v>
+        <v>12355201022.85185</v>
       </c>
       <c r="F75">
-        <v>4726625443.948874</v>
+        <v>10356610211.13953</v>
       </c>
       <c r="G75">
-        <v>582062570.2990532</v>
+        <v>1092508967.298548</v>
       </c>
       <c r="H75">
         <v>0</v>
       </c>
       <c r="I75">
-        <v>20.2400000003771</v>
+        <v>95.24000000037711</v>
       </c>
       <c r="J75">
-        <v>786.3899999998921</v>
+        <v>859.3899999998921</v>
       </c>
       <c r="K75">
-        <v>94.33999999965157</v>
+        <v>110.3399999996516</v>
       </c>
       <c r="L75">
-        <v>36083098.8023152</v>
+        <v>450619749.0523152</v>
       </c>
       <c r="M75">
-        <v>9324782.539999992</v>
+        <v>102548052.85</v>
       </c>
       <c r="N75">
-        <v>747362661.9774299</v>
+        <v>1998590811.71232</v>
       </c>
     </row>
     <row r="76">
@@ -4209,10 +4209,10 @@
         </is>
       </c>
       <c r="E78">
-        <v>169154557.57</v>
+        <v>161894277.84</v>
       </c>
       <c r="F78">
-        <v>76663005.43000001</v>
+        <v>73032865.57000001</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -4221,7 +4221,7 @@
         <v>0</v>
       </c>
       <c r="I78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J78">
         <v>0</v>
@@ -4230,13 +4230,13 @@
         <v>0</v>
       </c>
       <c r="L78">
-        <v>89587440.25</v>
+        <v>88861412.27</v>
       </c>
       <c r="M78">
-        <v>2904111.889999998</v>
+        <v>-2.561137080192566e-09</v>
       </c>
       <c r="N78">
-        <v>92491552.14</v>
+        <v>88861412.27</v>
       </c>
     </row>
     <row r="79">
@@ -4259,10 +4259,10 @@
         </is>
       </c>
       <c r="E79">
-        <v>3240636458.01</v>
+        <v>3220476932.44</v>
       </c>
       <c r="F79">
-        <v>1409038860.34</v>
+        <v>1397980113.41</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -4271,7 +4271,7 @@
         <v>0</v>
       </c>
       <c r="I79">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J79">
         <v>0</v>
@@ -4280,13 +4280,13 @@
         <v>0</v>
       </c>
       <c r="L79">
-        <v>1825491755.8</v>
+        <v>1822496819.03</v>
       </c>
       <c r="M79">
-        <v>6105841.870000007</v>
+        <v>6.410118658095598e-09</v>
       </c>
       <c r="N79">
-        <v>1831597597.67</v>
+        <v>1822496819.03</v>
       </c>
     </row>
     <row r="80">
@@ -4309,34 +4309,34 @@
         </is>
       </c>
       <c r="E80">
-        <v>1013927437.11</v>
+        <v>362832444.08</v>
       </c>
       <c r="F80">
-        <v>712640573.8100001</v>
+        <v>165871517.11</v>
       </c>
       <c r="G80">
-        <v>53587179.74</v>
+        <v>0</v>
       </c>
       <c r="H80">
         <v>0</v>
       </c>
       <c r="I80">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J80">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K80">
         <v>0</v>
       </c>
       <c r="L80">
-        <v>223798720.01</v>
+        <v>196960926.97</v>
       </c>
       <c r="M80">
-        <v>33862489.8</v>
+        <v>-7.566995918750763e-10</v>
       </c>
       <c r="N80">
-        <v>301286863.3</v>
+        <v>196960926.97</v>
       </c>
     </row>
     <row r="81">
@@ -4359,10 +4359,10 @@
         </is>
       </c>
       <c r="E81">
-        <v>400264694.16</v>
+        <v>396637347.13</v>
       </c>
       <c r="F81">
-        <v>171338090.51</v>
+        <v>168798947.59</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -4380,13 +4380,13 @@
         <v>0</v>
       </c>
       <c r="L81">
-        <v>228926603.65</v>
+        <v>227838399.54</v>
       </c>
       <c r="M81">
-        <v>-2.299202606081963e-09</v>
+        <v>-2.12457962334156e-09</v>
       </c>
       <c r="N81">
-        <v>228926603.65</v>
+        <v>227838399.54</v>
       </c>
     </row>
     <row r="82">
@@ -4409,34 +4409,34 @@
         </is>
       </c>
       <c r="E82">
-        <v>1314258108.86</v>
+        <v>637025209.74</v>
       </c>
       <c r="F82">
-        <v>856159285.9299999</v>
+        <v>314827758.3</v>
       </c>
       <c r="G82">
-        <v>46036618.05</v>
+        <v>1609771.33</v>
       </c>
       <c r="H82">
         <v>0</v>
       </c>
       <c r="I82">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="J82">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K82">
         <v>0</v>
       </c>
       <c r="L82">
-        <v>319014019.07</v>
+        <v>299071694.82</v>
       </c>
       <c r="M82">
-        <v>64225690.60000001</v>
+        <v>18693516.58000001</v>
       </c>
       <c r="N82">
-        <v>458098822.93</v>
+        <v>322197451.44</v>
       </c>
     </row>
     <row r="83">
@@ -4459,34 +4459,34 @@
         </is>
       </c>
       <c r="E83">
-        <v>6990879136.159761</v>
+        <v>10559412254.12976</v>
       </c>
       <c r="F83">
-        <v>5625966995.495073</v>
+        <v>8618128912.915073</v>
       </c>
       <c r="G83">
-        <v>1122498069.445394</v>
+        <v>1387013481.145394</v>
       </c>
       <c r="H83">
         <v>0</v>
       </c>
       <c r="I83">
-        <v>345.0999999999245</v>
+        <v>417.0999999999245</v>
       </c>
       <c r="J83">
-        <v>279</v>
+        <v>608</v>
       </c>
       <c r="K83">
-        <v>207.5</v>
+        <v>231.5</v>
       </c>
       <c r="L83">
-        <v>73581669.76680362</v>
+        <v>141429295.1068036</v>
       </c>
       <c r="M83">
-        <v>57002993.01</v>
+        <v>206888156.67</v>
       </c>
       <c r="N83">
-        <v>1364912140.664688</v>
+        <v>1941283341.214688</v>
       </c>
     </row>
     <row r="84">
@@ -4509,34 +4509,34 @@
         </is>
       </c>
       <c r="E84">
-        <v>27818044906.69865</v>
+        <v>21811066703.48</v>
       </c>
       <c r="F84">
-        <v>20241663003.27314</v>
+        <v>15880398304.34</v>
       </c>
       <c r="G84">
-        <v>802179948.4155096</v>
+        <v>492853590.9</v>
       </c>
       <c r="H84">
         <v>0</v>
       </c>
       <c r="I84">
-        <v>253</v>
+        <v>163</v>
       </c>
       <c r="J84">
-        <v>1033</v>
+        <v>702</v>
       </c>
       <c r="K84">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="L84">
-        <v>4115749407.11</v>
+        <v>3066607881.68</v>
       </c>
       <c r="M84">
-        <v>270424546.3399999</v>
+        <v>120539382.68</v>
       </c>
       <c r="N84">
-        <v>7576381903.425509</v>
+        <v>5930668399.14</v>
       </c>
     </row>
     <row r="85">
@@ -4559,10 +4559,10 @@
         </is>
       </c>
       <c r="E85">
-        <v>4652846956.15</v>
+        <v>5444677666.98</v>
       </c>
       <c r="F85">
-        <v>2810263265.87</v>
+        <v>3208888561.58</v>
       </c>
       <c r="G85">
         <v>333243353.415</v>
@@ -4571,7 +4571,7 @@
         <v>0</v>
       </c>
       <c r="I85">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="J85">
         <v>0</v>
@@ -4580,13 +4580,13 @@
         <v>80.5</v>
       </c>
       <c r="L85">
-        <v>1437337325.175</v>
+        <v>1774894574.215</v>
       </c>
       <c r="M85">
-        <v>109565036.1</v>
+        <v>165213202.18</v>
       </c>
       <c r="N85">
-        <v>1842583690.28</v>
+        <v>2235789105.4</v>
       </c>
     </row>
     <row r="86">
@@ -4609,34 +4609,34 @@
         </is>
       </c>
       <c r="E86">
-        <v>2357446342.92732</v>
+        <v>4612832586.10597</v>
       </c>
       <c r="F86">
-        <v>2052148966.825687</v>
+        <v>3904435000.618827</v>
       </c>
       <c r="G86">
-        <v>230308951.6509269</v>
+        <v>373133923.9264365</v>
       </c>
       <c r="H86">
         <v>0</v>
       </c>
       <c r="I86">
-        <v>10.90000000007554</v>
+        <v>49.90000000007554</v>
       </c>
       <c r="J86">
-        <v>391</v>
+        <v>408</v>
       </c>
       <c r="K86">
-        <v>48.5</v>
+        <v>49.5</v>
       </c>
       <c r="L86">
-        <v>19768602.31319637</v>
+        <v>188011429.8431964</v>
       </c>
       <c r="M86">
-        <v>2331608.129999998</v>
+        <v>35088059.62999999</v>
       </c>
       <c r="N86">
-        <v>305297376.1016334</v>
+        <v>708397585.487143</v>
       </c>
     </row>
     <row r="87">

</xml_diff>